<commit_message>
EXPORT aggiunto controller autorizzaione
</commit_message>
<xml_diff>
--- a/functions/export/src/40/F023588-M074Q114.xlsx
+++ b/functions/export/src/40/F023588-M074Q114.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
   <si>
     <t>ARTICOLO:</t>
   </si>
@@ -167,6 +167,27 @@
     <t>ORLATURA</t>
   </si>
   <si>
+    <t>LOGO</t>
+  </si>
+  <si>
+    <t>LVTI0029-0000</t>
+  </si>
+  <si>
+    <t>TIMBRO A FUOCO FERRAGAMO 50MM SU LINGUETTA</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>TIMBRO FOD</t>
+  </si>
+  <si>
+    <t>NT0001-0605</t>
+  </si>
+  <si>
+    <t>NASTRO X TIMBRO - H2 CM ARGENTO 7500</t>
+  </si>
+  <si>
     <t>FILO</t>
   </si>
   <si>
@@ -269,9 +290,6 @@
     <t>ART.A6949 / PUNTALE MAT. P124 (CASSINA GANC UOMO)</t>
   </si>
   <si>
-    <t>PA</t>
-  </si>
-  <si>
     <t>CONT.ORL</t>
   </si>
   <si>
@@ -300,6 +318,12 @@
   </si>
   <si>
     <t>AQUAGUM M/313 BOX BIANCO</t>
+  </si>
+  <si>
+    <t>AUTORIZZAZIONE:</t>
+  </si>
+  <si>
+    <t>Autorizzazione n° ITOPOIT01600002022-D-ROD99798 del 08/03/2022 Agenzia delle Dogane e Monopoli di Lecce</t>
   </si>
 </sst>
 </file>
@@ -341,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -349,14 +373,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,13 +701,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A21" sqref="A21:F21"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="75.41" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="3.428" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="8.141" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -679,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5045</v>
+        <v>1559</v>
       </c>
       <c r="F2"/>
     </row>
@@ -688,7 +740,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>122</v>
+        <v>269</v>
       </c>
       <c r="F3"/>
     </row>
@@ -742,7 +794,7 @@
         <v>0.08</v>
       </c>
       <c r="F7">
-        <v>9.76</v>
+        <v>21.52</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -762,7 +814,7 @@
         <v>0.18</v>
       </c>
       <c r="F8">
-        <v>21.96</v>
+        <v>48.42</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -782,7 +834,7 @@
         <v>0.13</v>
       </c>
       <c r="F9">
-        <v>15.86</v>
+        <v>34.97</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -802,7 +854,7 @@
         <v>0.128</v>
       </c>
       <c r="F10">
-        <v>15.62</v>
+        <v>34.43</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -822,7 +874,7 @@
         <v>0.035</v>
       </c>
       <c r="F11">
-        <v>4.27</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -842,7 +894,7 @@
         <v>0.035</v>
       </c>
       <c r="F12">
-        <v>4.27</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -862,7 +914,7 @@
         <v>0.016</v>
       </c>
       <c r="F13">
-        <v>1.95</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -882,7 +934,7 @@
         <v>0.04</v>
       </c>
       <c r="F14">
-        <v>4.88</v>
+        <v>10.76</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -902,7 +954,7 @@
         <v>0.02</v>
       </c>
       <c r="F15">
-        <v>2.44</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -922,7 +974,7 @@
         <v>0.115</v>
       </c>
       <c r="F16">
-        <v>14.03</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -942,7 +994,7 @@
         <v>0.025</v>
       </c>
       <c r="F17">
-        <v>3.05</v>
+        <v>6.73</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -962,7 +1014,7 @@
         <v>0.016</v>
       </c>
       <c r="F18">
-        <v>1.95</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -982,7 +1034,7 @@
         <v>0.017</v>
       </c>
       <c r="F19">
-        <v>2.07</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1002,7 +1054,7 @@
         <v>0.023</v>
       </c>
       <c r="F20">
-        <v>2.81</v>
+        <v>6.19</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1026,298 +1078,298 @@
         <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="E22">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1708.0</v>
+        <v>269.0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
         <v>24</v>
       </c>
       <c r="E23">
-        <v>7</v>
+        <v>0.07</v>
       </c>
       <c r="F23">
-        <v>854.0</v>
+        <v>18.83</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F24">
-        <v>366.0</v>
+        <v>3766.0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
       <c r="E25">
-        <v>1.5</v>
+        <v>7</v>
       </c>
       <c r="F25">
-        <v>183.0</v>
+        <v>1883.0</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>976.0</v>
+        <v>807.0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
         <v>24</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="F27">
-        <v>488.0</v>
+        <v>403.5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="E28">
-        <v>0.014</v>
+        <v>8</v>
       </c>
       <c r="F28">
-        <v>1.71</v>
+        <v>2152.0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" t="s">
-        <v>66</v>
-      </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="E29">
-        <v>0.001</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>0.12</v>
+        <v>1076.0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E30">
-        <v>0.001</v>
+        <v>0.014</v>
       </c>
       <c r="F30">
-        <v>0.12</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
         <v>71</v>
       </c>
-      <c r="C31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>24</v>
-      </c>
       <c r="E31">
-        <v>0.3</v>
+        <v>0.001</v>
       </c>
       <c r="F31">
-        <v>36.6</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="E32">
-        <v>1.5</v>
+        <v>0.001</v>
       </c>
       <c r="F32">
-        <v>183.0</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D33" t="s">
         <v>24</v>
       </c>
       <c r="E33">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="F33">
-        <v>85.4</v>
+        <v>80.7</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
         <v>24</v>
       </c>
       <c r="E34">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
       <c r="F34">
-        <v>24.4</v>
+        <v>403.5</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
         <v>24</v>
       </c>
       <c r="E35">
-        <v>2.8</v>
+        <v>0.7</v>
       </c>
       <c r="F35">
-        <v>341.6</v>
+        <v>188.3</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F36">
-        <v>122.0</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>86</v>
@@ -1326,13 +1378,13 @@
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="F37">
-        <v>122.0</v>
+        <v>753.2</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1346,36 +1398,91 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E38">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <v>2928.0</v>
+        <v>269.0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
         <v>92</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>93</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>269.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>94</v>
       </c>
-      <c r="D39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39">
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40">
+        <v>24</v>
+      </c>
+      <c r="F40">
+        <v>6456.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41">
         <v>0.01</v>
       </c>
-      <c r="F39">
-        <v>1.22</v>
-      </c>
+      <c r="F41">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="B44:F44"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
EXPORT gestione documenti vuoti
</commit_message>
<xml_diff>
--- a/functions/export/src/40/F023588-M074Q114.xlsx
+++ b/functions/export/src/40/F023588-M074Q114.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>ARTICOLO:</t>
   </si>
@@ -167,129 +167,111 @@
     <t>ORLATURA</t>
   </si>
   <si>
-    <t>LOGO</t>
-  </si>
-  <si>
-    <t>LVTI0029-0000</t>
-  </si>
-  <si>
-    <t>TIMBRO A FUOCO FERRAGAMO 50MM SU LINGUETTA</t>
+    <t>FILO</t>
+  </si>
+  <si>
+    <t>FIS0300004000</t>
+  </si>
+  <si>
+    <t>FILO 30 (PZ) SERAFIL 4000</t>
+  </si>
+  <si>
+    <t>FIS0400004000</t>
+  </si>
+  <si>
+    <t>FILO 40 (PZ) SERAFIL 4000</t>
+  </si>
+  <si>
+    <t>FIS0200000416</t>
+  </si>
+  <si>
+    <t>FILO 20 (PZ) SERAFIL 416</t>
+  </si>
+  <si>
+    <t>FIS0400000416</t>
+  </si>
+  <si>
+    <t>FILO 40 (PZ) SERAFIL 416</t>
+  </si>
+  <si>
+    <t>FIS0600004000</t>
+  </si>
+  <si>
+    <t>FILO 60 (PZ) SERAFIL 4000</t>
+  </si>
+  <si>
+    <t>COLLA</t>
+  </si>
+  <si>
+    <t>GEGE00150000</t>
+  </si>
+  <si>
+    <t>VULKAPRENE 878</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>MCCO00140102</t>
+  </si>
+  <si>
+    <t>SAR 700 NATURALE</t>
+  </si>
+  <si>
+    <t>TINTA</t>
+  </si>
+  <si>
+    <t>MCTI9999NERO</t>
+  </si>
+  <si>
+    <t>TINTA TINGIBORDI NERO</t>
+  </si>
+  <si>
+    <t>RINF.ORL.</t>
+  </si>
+  <si>
+    <t>RN3050-0999</t>
+  </si>
+  <si>
+    <t>FETTUCCIA NYLON MM 30X50 NERO</t>
+  </si>
+  <si>
+    <t>BI0650-0000</t>
+  </si>
+  <si>
+    <t>BIADESIVO MM 6X50</t>
+  </si>
+  <si>
+    <t>RM0450-0999</t>
+  </si>
+  <si>
+    <t>FETTUCCIA MISTO NYLON/COTONE MM 4X50 NERO</t>
+  </si>
+  <si>
+    <t>RN2050-0999</t>
+  </si>
+  <si>
+    <t>FETTUCCIA NYLON MM 20X50 NERO</t>
+  </si>
+  <si>
+    <t>AL1000-0000</t>
+  </si>
+  <si>
+    <t>STRINGA X ALLACCIATURA ART. TOMAIA (1 RTL/500 MT)</t>
+  </si>
+  <si>
+    <t>PUNT.ORL.</t>
+  </si>
+  <si>
+    <t>PU6949</t>
+  </si>
+  <si>
+    <t>ART.A6949 / PUNTALE MAT. P124 (CASSINA GANC UOMO)</t>
   </si>
   <si>
     <t>PA</t>
   </si>
   <si>
-    <t>TIMBRO FOD</t>
-  </si>
-  <si>
-    <t>NT0001-0605</t>
-  </si>
-  <si>
-    <t>NASTRO X TIMBRO - H2 CM ARGENTO 7500</t>
-  </si>
-  <si>
-    <t>FILO</t>
-  </si>
-  <si>
-    <t>FIS0300004000</t>
-  </si>
-  <si>
-    <t>FILO 30 (PZ) SERAFIL 4000</t>
-  </si>
-  <si>
-    <t>FIS0400004000</t>
-  </si>
-  <si>
-    <t>FILO 40 (PZ) SERAFIL 4000</t>
-  </si>
-  <si>
-    <t>FIS0200000416</t>
-  </si>
-  <si>
-    <t>FILO 20 (PZ) SERAFIL 416</t>
-  </si>
-  <si>
-    <t>FIS0400000416</t>
-  </si>
-  <si>
-    <t>FILO 40 (PZ) SERAFIL 416</t>
-  </si>
-  <si>
-    <t>FIS0600004000</t>
-  </si>
-  <si>
-    <t>FILO 60 (PZ) SERAFIL 4000</t>
-  </si>
-  <si>
-    <t>COLLA</t>
-  </si>
-  <si>
-    <t>GEGE00150000</t>
-  </si>
-  <si>
-    <t>VULKAPRENE 878</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>MCCO00140102</t>
-  </si>
-  <si>
-    <t>SAR 700 NATURALE</t>
-  </si>
-  <si>
-    <t>TINTA</t>
-  </si>
-  <si>
-    <t>MCTI9999NERO</t>
-  </si>
-  <si>
-    <t>TINTA TINGIBORDI NERO</t>
-  </si>
-  <si>
-    <t>RINF.ORL.</t>
-  </si>
-  <si>
-    <t>RN3050-0999</t>
-  </si>
-  <si>
-    <t>FETTUCCIA NYLON MM 30X50 NERO</t>
-  </si>
-  <si>
-    <t>BI0650-0000</t>
-  </si>
-  <si>
-    <t>BIADESIVO MM 6X50</t>
-  </si>
-  <si>
-    <t>RM0450-0999</t>
-  </si>
-  <si>
-    <t>FETTUCCIA MISTO NYLON/COTONE MM 4X50 NERO</t>
-  </si>
-  <si>
-    <t>RN2050-0999</t>
-  </si>
-  <si>
-    <t>FETTUCCIA NYLON MM 20X50 NERO</t>
-  </si>
-  <si>
-    <t>AL1000-0000</t>
-  </si>
-  <si>
-    <t>STRINGA X ALLACCIATURA ART. TOMAIA (1 RTL/500 MT)</t>
-  </si>
-  <si>
-    <t>PUNT.ORL.</t>
-  </si>
-  <si>
-    <t>PU6949</t>
-  </si>
-  <si>
-    <t>ART.A6949 / PUNTALE MAT. P124 (CASSINA GANC UOMO)</t>
-  </si>
-  <si>
     <t>CONT.ORL</t>
   </si>
   <si>
@@ -318,12 +300,6 @@
   </si>
   <si>
     <t>AQUAGUM M/313 BOX BIANCO</t>
-  </si>
-  <si>
-    <t>AUTORIZZAZIONE:</t>
-  </si>
-  <si>
-    <t>Autorizzazione n° ITOPOIT01600002022-D-ROD99798 del 08/03/2022 Agenzia delle Dogane e Monopoli di Lecce</t>
   </si>
 </sst>
 </file>
@@ -365,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -373,34 +349,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,10 +657,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="A21" sqref="A21:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1559</v>
+        <v>4569</v>
       </c>
       <c r="F2"/>
     </row>
@@ -740,7 +696,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>269</v>
+        <v>125</v>
       </c>
       <c r="F3"/>
     </row>
@@ -794,7 +750,7 @@
         <v>0.08</v>
       </c>
       <c r="F7">
-        <v>21.52</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -814,7 +770,7 @@
         <v>0.18</v>
       </c>
       <c r="F8">
-        <v>48.42</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -834,7 +790,7 @@
         <v>0.13</v>
       </c>
       <c r="F9">
-        <v>34.97</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -854,7 +810,7 @@
         <v>0.128</v>
       </c>
       <c r="F10">
-        <v>34.43</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -874,7 +830,7 @@
         <v>0.035</v>
       </c>
       <c r="F11">
-        <v>9.42</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -894,7 +850,7 @@
         <v>0.035</v>
       </c>
       <c r="F12">
-        <v>9.42</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -914,7 +870,7 @@
         <v>0.016</v>
       </c>
       <c r="F13">
-        <v>4.3</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -934,7 +890,7 @@
         <v>0.04</v>
       </c>
       <c r="F14">
-        <v>10.76</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -954,7 +910,7 @@
         <v>0.02</v>
       </c>
       <c r="F15">
-        <v>5.38</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -974,7 +930,7 @@
         <v>0.115</v>
       </c>
       <c r="F16">
-        <v>30.94</v>
+        <v>14.38</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -994,7 +950,7 @@
         <v>0.025</v>
       </c>
       <c r="F17">
-        <v>6.73</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1014,7 +970,7 @@
         <v>0.016</v>
       </c>
       <c r="F18">
-        <v>4.3</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1034,7 +990,7 @@
         <v>0.017</v>
       </c>
       <c r="F19">
-        <v>4.57</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1054,7 +1010,7 @@
         <v>0.023</v>
       </c>
       <c r="F20">
-        <v>6.19</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1078,298 +1034,298 @@
         <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F22">
-        <v>269.0</v>
+        <v>1750.0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
       <c r="D23" t="s">
         <v>24</v>
       </c>
       <c r="E23">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="F23">
-        <v>18.83</v>
+        <v>875.0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
       </c>
       <c r="E24">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>3766.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>1.5</v>
       </c>
       <c r="F25">
-        <v>1883.0</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>807.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>24</v>
       </c>
       <c r="E27">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F27">
-        <v>403.5</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>0.014</v>
       </c>
       <c r="F28">
-        <v>2152.0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>0.001</v>
       </c>
       <c r="F29">
-        <v>1076.0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>69</v>
       </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E30">
-        <v>0.014</v>
+        <v>0.001</v>
       </c>
       <c r="F30">
-        <v>3.77</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
         <v>72</v>
       </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="E31">
-        <v>0.001</v>
+        <v>0.3</v>
       </c>
       <c r="F31">
-        <v>0.27</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
         <v>74</v>
       </c>
-      <c r="B32" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="E32">
-        <v>0.001</v>
+        <v>1.5</v>
       </c>
       <c r="F32">
-        <v>0.27</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
         <v>24</v>
       </c>
       <c r="E33">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="F33">
-        <v>80.7</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
         <v>77</v>
       </c>
-      <c r="B34" t="s">
-        <v>80</v>
-      </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
         <v>24</v>
       </c>
       <c r="E34">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="F34">
-        <v>403.5</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
         <v>24</v>
       </c>
       <c r="E35">
-        <v>0.7</v>
+        <v>2.8</v>
       </c>
       <c r="F35">
-        <v>188.3</v>
+        <v>350.0</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s">
         <v>84</v>
       </c>
-      <c r="C36" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
       <c r="E36">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>53.8</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
         <v>86</v>
@@ -1378,13 +1334,13 @@
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E37">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>753.2</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1398,91 +1354,36 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F38">
-        <v>269.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="F39">
-        <v>269.0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" t="s">
-        <v>97</v>
-      </c>
-      <c r="E40">
-        <v>24</v>
-      </c>
-      <c r="F40">
-        <v>6456.0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41">
-        <v>0.01</v>
-      </c>
-      <c r="F41">
-        <v>2.69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+        <v>1.25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="B44:F44"/>
-  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>